<commit_message>
Enchanting completed - hooray!
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Enchanting/Runes.xlsx
+++ b/CoreRulebook/Data/Enchanting/Runes.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">p</t>
   </si>
   <si>
-    <t xml:space="preserve">Contain</t>
+    <t xml:space="preserve">The containment rune: used when the enchantment involves restraining or containing the subject matter within the object. </t>
   </si>
   <si>
     <t xml:space="preserve">animus</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">\y</t>
   </si>
   <si>
-    <t xml:space="preserve">Astral</t>
+    <t xml:space="preserve">The Astral rune: the domain of the spirit, the extraplanar and the Unliving. </t>
   </si>
   <si>
     <t xml:space="preserve">velox</t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">\D</t>
   </si>
   <si>
-    <t xml:space="preserve">Protect</t>
+    <t xml:space="preserve">The protective rune: used to protect the subject from harm, extend its lifetime or prevent the degredation of itself or others</t>
   </si>
   <si>
     <t xml:space="preserve">aqua</t>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">\dh</t>
   </si>
   <si>
-    <t xml:space="preserve">Water</t>
+    <t xml:space="preserve">The Water rune: the domain of water, ice and other fluids. </t>
   </si>
   <si>
     <t xml:space="preserve">lentus</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">\belgthor</t>
   </si>
   <si>
-    <t xml:space="preserve">Learn</t>
+    <t xml:space="preserve">The perception rune: used to extend or nullify the senses, and to aid in the perception and understanding of the subject. </t>
   </si>
   <si>
     <t xml:space="preserve">arbor</t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">Y</t>
   </si>
   <si>
-    <t xml:space="preserve">Nature</t>
+    <t xml:space="preserve">The Nature rune: the domain of plants, soil, leaves and the natural world.</t>
   </si>
   <si>
     <t xml:space="preserve">aeternum</t>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">m</t>
   </si>
   <si>
-    <t xml:space="preserve">Create</t>
+    <t xml:space="preserve">The creation rune: used to summon something from nothing, to create an entirely new example of the subject. </t>
   </si>
   <si>
     <t xml:space="preserve">belua</t>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">\tvimadur</t>
   </si>
   <si>
-    <t xml:space="preserve">Beasts</t>
+    <t xml:space="preserve">The Beast rune: the domain of non-sapient beasts and animals</t>
   </si>
   <si>
     <t xml:space="preserve">imperum</t>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">\Pdots</t>
   </si>
   <si>
-    <t xml:space="preserve">Control</t>
+    <t xml:space="preserve">The manipulation rune: used to allow the manipulation or control of the subject, without altering its nature. </t>
   </si>
   <si>
     <t xml:space="preserve">caelus</t>
@@ -163,7 +163,7 @@
     <t xml:space="preserve">\x</t>
   </si>
   <si>
-    <t xml:space="preserve">Air</t>
+    <t xml:space="preserve">The Air rune: the domain of wind, storms and flight. </t>
   </si>
   <si>
     <t xml:space="preserve">muto</t>
@@ -172,7 +172,7 @@
     <t xml:space="preserve">\tring</t>
   </si>
   <si>
-    <t xml:space="preserve">Transform</t>
+    <t xml:space="preserve">The transformation rune: used to alter the nature and form of the subject.</t>
   </si>
   <si>
     <t xml:space="preserve">fabula</t>
@@ -181,7 +181,7 @@
     <t xml:space="preserve">\thth</t>
   </si>
   <si>
-    <t xml:space="preserve">Arcane</t>
+    <t xml:space="preserve">The Arcane rune: the domain of pure magical energies, spells and power. </t>
   </si>
   <si>
     <t xml:space="preserve">perdero</t>
@@ -190,7 +190,7 @@
     <t xml:space="preserve">y</t>
   </si>
   <si>
-    <t xml:space="preserve">Destroy</t>
+    <t xml:space="preserve">The destruction rune: used to project negative energies which degrade, destroy, damage and otherwise break and reduce the subject.  </t>
   </si>
   <si>
     <t xml:space="preserve">hominus</t>
@@ -199,7 +199,7 @@
     <t xml:space="preserve">x</t>
   </si>
   <si>
-    <t xml:space="preserve">Bodies</t>
+    <t xml:space="preserve">The Body rune: the domain of sapient creatures and their physical form. </t>
   </si>
   <si>
     <t xml:space="preserve">porto</t>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">\T</t>
   </si>
   <si>
-    <t xml:space="preserve">Transmit</t>
+    <t xml:space="preserve">The transmission rune: used to project or transfer the subject over large distances</t>
   </si>
   <si>
     <t xml:space="preserve">ignis</t>
@@ -217,7 +217,7 @@
     <t xml:space="preserve">F</t>
   </si>
   <si>
-    <t xml:space="preserve">Fire</t>
+    <t xml:space="preserve">The Fire rune: the domain of flames, lava, and heat. </t>
   </si>
   <si>
     <t xml:space="preserve">sarco</t>
@@ -226,7 +226,7 @@
     <t xml:space="preserve">o</t>
   </si>
   <si>
-    <t xml:space="preserve">Repair</t>
+    <t xml:space="preserve">The rebuilding rune: used to repair, heal and restore the subject. </t>
   </si>
   <si>
     <t xml:space="preserve">locus</t>
@@ -235,7 +235,7 @@
     <t xml:space="preserve">\e</t>
   </si>
   <si>
-    <t xml:space="preserve">Space</t>
+    <t xml:space="preserve">The Space rune: the domain of length, volume, speed and gravity. </t>
   </si>
   <si>
     <t xml:space="preserve">lux</t>
@@ -244,7 +244,7 @@
     <t xml:space="preserve">w</t>
   </si>
   <si>
-    <t xml:space="preserve">Light</t>
+    <t xml:space="preserve">The Light rune: the domain of light, darkness and illusions. </t>
   </si>
   <si>
     <t xml:space="preserve">morbus</t>
@@ -253,7 +253,7 @@
     <t xml:space="preserve">\rdot</t>
   </si>
   <si>
-    <t xml:space="preserve">Toxins</t>
+    <t xml:space="preserve">The Cursed rune: the domain of poisons, curses, diseases and other evil and unpleasant things. </t>
   </si>
   <si>
     <t xml:space="preserve">pondus</t>
@@ -262,7 +262,7 @@
     <t xml:space="preserve">\Y</t>
   </si>
   <si>
-    <t xml:space="preserve">Matter</t>
+    <t xml:space="preserve">The Matter rune: the domain of mass, objects and the physical world. </t>
   </si>
   <si>
     <t xml:space="preserve">sensus</t>
@@ -271,7 +271,7 @@
     <t xml:space="preserve">s</t>
   </si>
   <si>
-    <t xml:space="preserve">Mind</t>
+    <t xml:space="preserve">The Mind rune: the domain of consciousness, dreams and the brain. </t>
   </si>
   <si>
     <t xml:space="preserve">tempus</t>
@@ -280,7 +280,7 @@
     <t xml:space="preserve">E</t>
   </si>
   <si>
-    <t xml:space="preserve">Time</t>
+    <t xml:space="preserve">The Time rune: the domain of the past, the future </t>
   </si>
   <si>
     <t xml:space="preserve">terra</t>
@@ -289,7 +289,7 @@
     <t xml:space="preserve">\arlaug</t>
   </si>
   <si>
-    <t xml:space="preserve">Earth</t>
+    <t xml:space="preserve">The Earth rune: the domain of earth, clay, rocks and stone. </t>
   </si>
 </sst>
 </file>
@@ -304,6 +304,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -363,9 +364,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -376,14 +385,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -393,329 +406,426 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="37.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.54"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="J3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="L3" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="H4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="J4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="K4" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="L4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="F5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="G5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="H5" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="J5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="K5" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="L5" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="F6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="G6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="H6" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="J6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="K6" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="0" t="s">
+      <c r="L6" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="F7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="G7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="H7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="J7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="K7" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="0" t="s">
+      <c r="L7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="F8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="G8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="H8" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="J8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="K8" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="0" t="s">
+      <c r="L8" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="F9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="G9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="H9" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="J9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="K9" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="2" t="s">
+      <c r="L9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="F10" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="G10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="H10" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="J10" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="K10" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="0" t="s">
+      <c r="L10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="F11" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="G11" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="H11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="J11" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="K11" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G12" s="0" t="s">
+      <c r="L11" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I12" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="J12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="K12" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G13" s="0" t="s">
+      <c r="L12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I13" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="J13" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="K13" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G14" s="0" t="s">
+      <c r="L13" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I14" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="J14" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="K14" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G15" s="0" t="s">
+      <c r="L14" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I15" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="J15" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="K15" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G16" s="0" t="s">
+      <c r="L15" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I16" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="J16" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="K16" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G17" s="0" t="s">
+      <c r="L16" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I17" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="J17" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I17" s="0" t="s">
+      <c r="K17" s="5" t="s">
         <v>89</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:K1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>